<commit_message>
[MS-WDVMODUU]: Update RS according to lastest version TD
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WDVMODUU/MS-WDVMODUU_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WDVMODUU/MS-WDVMODUU_RequirementSpecification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\InteropO15Dev\TestSuites\SharePoint\Platinum\SPSPTS_Dev\SharePoint Server Protocol Test Suites\Docs\MS-WDVMODUU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites2\SharePoint\Docs\MS-WDVMODUU\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$132</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="329">
   <si>
     <t>Req ID</t>
   </si>
@@ -942,9 +942,6 @@
 Version-Number = "1.0"</t>
   </si>
   <si>
-    <t>[In MS-BinDiff Header] Because the server ignores this header, there are no usage specifications for this header.</t>
-  </si>
-  <si>
     <t>[In X-Office-Version Header] A WebDAV client SHOULD NOT include the X-Office-Version header in any HTTP 1.1 requests.&lt;8&gt;</t>
   </si>
   <si>
@@ -976,9 +973,6 @@
     <t>[In Repl:collblob Element] The Repl:collblob element MUST NOT appear except within the Repl:repl XML element collection.</t>
   </si>
   <si>
-    <t>[In Repl:collblob Element] The Repl:collblob element usage is specified in section 3.1.4.9 and section 3.2.4.2.</t>
-  </si>
-  <si>
     <t>[In Repl:repl Element Collection] The Repl:repl XML element collection MUST contain a single Repl:collblob element, as specified in section 2.2.2.1).</t>
   </si>
   <si>
@@ -988,9 +982,6 @@
     <t>[In Repl:repl Element Collection] [This Repl:repl Element collection appears] within the multistatus element collection (section 2.2.2). &lt;!ELEMENT repl (collblob) &gt;</t>
   </si>
   <si>
-    <t>[In Repl:repl Element Collection] The Repl:repl element collection usage is specified in sections 3.1.4.9 and 3.2.4.2.</t>
-  </si>
-  <si>
     <t>[In Protocol Details] As specified in [RFC2518], WebDAV operates between a requester, or WebDAV client, and a responder, or WebDAV server.</t>
   </si>
   <si>
@@ -1033,9 +1024,6 @@
     <t>[In MS-Set-Repl-Uid Header] The MS-Set-Repl-Uid header is ignored by WebDAV servers.</t>
   </si>
   <si>
-    <t>[In MS-BinDiff Header] The MS-BinDiff header is ignored by WebDAV servers.</t>
-  </si>
-  <si>
     <t>[In X-Office-Version Header] The X-Office-Version header is ignored by WebDAV servers.</t>
   </si>
   <si>
@@ -1052,9 +1040,6 @@
   </si>
   <si>
     <t>[In Repl:collblob and Repl:repl] [When the server receives a PROPFIND request with the Repl:collblob element set to a timestamp, it includes a response element for each resource in the multistatus element that is a descendant of the Request-URI (limited by the Depth header specified in [RFC2518]) and that has changed according to the rule:] The resource was last modified later than 5 minutes before the timestamp.</t>
-  </si>
-  <si>
-    <t>[In Repl:collblob and Repl:repl] [When the server receives a PROPFIND request with the Repl:collblob element set to a timestamp, it includes a response element for each resource in the multistatus element that is a descendant of the Request-URI (limited by the Depth header specified in [RFC2518]) and that has changed according to the rule:] The resource is a descendant of a resource that has changed.</t>
   </si>
   <si>
     <t>[In Repl:collblob and Repl:repl] [When the server receives a PROPFIND request with the Repl:collblob element set to a timestamp] In addition, the server includes the Repl:repl element collection in the response as specified.
@@ -1100,9 +1085,6 @@
     <t>[In Appendix B: Product Behavior] Unless otherwise specified, the term MAY implies that the product does not follow the prescription.</t>
   </si>
   <si>
-    <t>[In Appendix B: Product Behavior] &lt;1&gt; Section 1.5:  Office 2007 SP1 system clients use MODUU extensions only against a Document Workspace site.</t>
-  </si>
-  <si>
     <t>[In Appendix B: Product Behavior] &lt;2&gt; Section 2.2.1.2:  Office 2007 SP1 system clients include the Moss-Uid header in GET, PUT, OPTIONS, MOVE, DELETE, MKCOL and PROPFIND requests, though Windows SharePoint Services 3.0 ignores it.</t>
   </si>
   <si>
@@ -1215,10 +1197,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In MS-BinDiff Header] [The reply of implementation does be the same whether MS-BinDiff header is included in the request or not.]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[In X-Office-Version Header] [The reply of implementation does be the same whether X-Office-Version header is included in the request or not.]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1240,12 +1218,66 @@
   </si>
   <si>
     <t>Open Specification Date:</t>
+  </si>
+  <si>
+    <t>[In MS-BinDiff Header] Because the server ignores this header unless it is included in an HTTP PUT request, there are no usage specifications for this header.</t>
+  </si>
+  <si>
+    <t>MS-WDVMODUU_R601</t>
+  </si>
+  <si>
+    <t>[In User-Agent Header] Because the server ignores this header, there are no usage specifications for this header.</t>
+  </si>
+  <si>
+    <t>[In Repl:collblob Element] The Repl:collblob element usage is specified in section 3.1.4.10 and section 3.2.4.2.</t>
+  </si>
+  <si>
+    <t>[In Repl:repl Element Collection] The Repl:repl element collection usage is specified in sections 3.1.4.10 and 3.2.4.2.</t>
+  </si>
+  <si>
+    <t>MS-WDVMODUU_R901</t>
+  </si>
+  <si>
+    <t>[In MS-BinDiff Header] [The reply of implementation does be the same whether MS-BinDiff header is included in the request or not.]</t>
+  </si>
+  <si>
+    <t>[In MS-BinDiff Header] The MS-BinDiff header is ignored by WebDAV servers unless it is included in an HTTP PUT request.</t>
+  </si>
+  <si>
+    <t>[In MS-BinDiff Header] If the MS-BinDiff header is included in an HTTP PUT request, the server MUST fail the request and response with a message containing HTTP status code "415 UNSUPPORTED MEDIA TYPE".</t>
+  </si>
+  <si>
+    <t>MS-WDVMODUU_R921</t>
+  </si>
+  <si>
+    <t>[In User-Agent Header] The User-Agent Header header is ignored by WebDAV servers.</t>
+  </si>
+  <si>
+    <t>MS-WDVMODUU_R922</t>
+  </si>
+  <si>
+    <t>[In User-Agent Header] The reply of implementation does be the same whether WebDAV header is included in the request or not.</t>
+  </si>
+  <si>
+    <t>MS-WDVMODUU_R921:p</t>
+  </si>
+  <si>
+    <t>Partially verified by derived requirement: MS-WDVMODUU_R922.</t>
+  </si>
+  <si>
+    <t>3.1.4.10</t>
+  </si>
+  <si>
+    <t>[In Repl:collblob and Repl:repl] [When the server receives a PROPFIND request with the Repl:collblob element set to a timestamp, it includes a response element for each resource in the multistatus element that is a descendant of the Request-URI (limited by the Depth header specified in [RFC2518]) and that has changed according to the rule:] The resource is a descendant of a resource that has changed later than or equal to 5 minutes before the timestamp.</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] &lt;1&gt; Section 1.5:  Microsoft Office 2007 Service Pack 1 (SP1) system clients use MODUU extensions only against a Document Workspace site.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -1511,21 +1543,6 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1549,6 +1566,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2066,8 +2098,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I128" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I128"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I132" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I132"/>
   <tableColumns count="9">
     <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -2189,6 +2221,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2224,6 +2273,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2401,28 +2467,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L130"/>
+  <dimension ref="A1:L134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -2432,7 +2498,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2446,138 +2512,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="29">
-        <v>2.7</v>
+        <v>5</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="F3" s="12">
-        <v>41185</v>
+        <v>42566</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -2590,12 +2656,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -2608,12 +2674,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -2626,12 +2692,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -2644,60 +2710,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -2806,7 +2872,7 @@
       </c>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="23" spans="1:12" s="23" customFormat="1">
       <c r="A23" s="22" t="s">
         <v>45</v>
       </c>
@@ -2831,7 +2897,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A24" s="22" t="s">
         <v>46</v>
       </c>
@@ -3006,7 +3072,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" ht="60">
+    <row r="31" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A31" s="22" t="s">
         <v>53</v>
       </c>
@@ -3181,7 +3247,7 @@
       </c>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9" ht="30">
+    <row r="38" spans="1:9">
       <c r="A38" s="30" t="s">
         <v>60</v>
       </c>
@@ -3713,8 +3779,8 @@
       <c r="B59" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="C59" s="32" t="s">
-        <v>227</v>
+      <c r="C59" s="20" t="s">
+        <v>311</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30" t="s">
@@ -3739,7 +3805,7 @@
         <v>162</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30" t="s">
@@ -3764,7 +3830,7 @@
         <v>162</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D61" s="30"/>
       <c r="E61" s="30" t="s">
@@ -3789,7 +3855,7 @@
         <v>162</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30" t="s">
@@ -3814,7 +3880,7 @@
         <v>162</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D63" s="30"/>
       <c r="E63" s="30" t="s">
@@ -3839,7 +3905,7 @@
         <v>163</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="30" t="s">
@@ -3857,14 +3923,14 @@
       <c r="I64" s="32"/>
     </row>
     <row r="65" spans="1:9" ht="45">
-      <c r="A65" s="30" t="s">
+      <c r="A65" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B65" s="31" t="s">
+      <c r="B65" s="24" t="s">
         <v>163</v>
       </c>
-      <c r="C65" s="32" t="s">
-        <v>233</v>
+      <c r="C65" s="20" t="s">
+        <v>232</v>
       </c>
       <c r="D65" s="30"/>
       <c r="E65" s="30" t="s">
@@ -3881,15 +3947,15 @@
       </c>
       <c r="I65" s="32"/>
     </row>
-    <row r="66" spans="1:9" ht="45">
+    <row r="66" spans="1:9" ht="30">
       <c r="A66" s="30" t="s">
-        <v>88</v>
+        <v>312</v>
       </c>
       <c r="B66" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="C66" s="32" t="s">
-        <v>234</v>
+        <v>163</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>313</v>
       </c>
       <c r="D66" s="30"/>
       <c r="E66" s="30" t="s">
@@ -3899,29 +3965,29 @@
         <v>6</v>
       </c>
       <c r="G66" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H66" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I66" s="32"/>
     </row>
     <row r="67" spans="1:9" ht="45">
       <c r="A67" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B67" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D67" s="30"/>
       <c r="E67" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F67" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G67" s="30" t="s">
         <v>15</v>
@@ -3931,15 +3997,15 @@
       </c>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" ht="30">
+    <row r="68" spans="1:9" ht="45">
       <c r="A68" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B68" s="31" t="s">
         <v>165</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30" t="s">
@@ -3958,13 +4024,13 @@
     </row>
     <row r="69" spans="1:9" ht="30">
       <c r="A69" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B69" s="31" t="s">
         <v>165</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D69" s="30"/>
       <c r="E69" s="30" t="s">
@@ -3974,22 +4040,22 @@
         <v>3</v>
       </c>
       <c r="G69" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H69" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9" ht="30">
+    <row r="70" spans="1:9">
       <c r="A70" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="C70" s="32" t="s">
-        <v>238</v>
+        <v>165</v>
+      </c>
+      <c r="C70" s="20" t="s">
+        <v>314</v>
       </c>
       <c r="D70" s="30"/>
       <c r="E70" s="30" t="s">
@@ -3999,97 +4065,97 @@
         <v>3</v>
       </c>
       <c r="G70" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H70" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I70" s="32"/>
     </row>
     <row r="71" spans="1:9" ht="30">
       <c r="A71" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B71" s="31" t="s">
         <v>166</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F71" s="30" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G71" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H71" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I71" s="32"/>
     </row>
     <row r="72" spans="1:9" ht="30">
       <c r="A72" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B72" s="31" t="s">
         <v>166</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D72" s="30"/>
       <c r="E72" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F72" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G72" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H72" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I72" s="32"/>
     </row>
     <row r="73" spans="1:9" ht="30">
       <c r="A73" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B73" s="31" t="s">
         <v>166</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D73" s="30"/>
       <c r="E73" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F73" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G73" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H73" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I73" s="32"/>
     </row>
     <row r="74" spans="1:9" ht="30">
       <c r="A74" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="C74" s="32" t="s">
-        <v>242</v>
+        <v>166</v>
+      </c>
+      <c r="C74" s="20" t="s">
+        <v>315</v>
       </c>
       <c r="D74" s="30"/>
       <c r="E74" s="30" t="s">
@@ -4108,13 +4174,13 @@
     </row>
     <row r="75" spans="1:9" ht="30">
       <c r="A75" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B75" s="31" t="s">
         <v>167</v>
       </c>
       <c r="C75" s="32" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D75" s="30"/>
       <c r="E75" s="30" t="s">
@@ -4131,22 +4197,22 @@
       </c>
       <c r="I75" s="32"/>
     </row>
-    <row r="76" spans="1:9" ht="30">
+    <row r="76" spans="1:9">
       <c r="A76" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B76" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C76" s="32" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D76" s="30"/>
       <c r="E76" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F76" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G76" s="30" t="s">
         <v>16</v>
@@ -4156,15 +4222,15 @@
       </c>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" ht="30">
       <c r="A77" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B77" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D77" s="30"/>
       <c r="E77" s="30" t="s">
@@ -4174,22 +4240,22 @@
         <v>6</v>
       </c>
       <c r="G77" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H77" s="30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I77" s="32"/>
     </row>
-    <row r="78" spans="1:9" ht="30">
+    <row r="78" spans="1:9">
       <c r="A78" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D78" s="30"/>
       <c r="E78" s="30" t="s">
@@ -4206,15 +4272,15 @@
       </c>
       <c r="I78" s="32"/>
     </row>
-    <row r="79" spans="1:9" ht="45">
+    <row r="79" spans="1:9">
       <c r="A79" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B79" s="31" t="s">
-        <v>31</v>
+        <v>170</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D79" s="30"/>
       <c r="E79" s="30" t="s">
@@ -4227,19 +4293,19 @@
         <v>15</v>
       </c>
       <c r="H79" s="30" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I79" s="32"/>
     </row>
-    <row r="80" spans="1:9" ht="45">
+    <row r="80" spans="1:9" ht="30">
       <c r="A80" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B80" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C80" s="32" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D80" s="30"/>
       <c r="E80" s="30" t="s">
@@ -4256,15 +4322,15 @@
       </c>
       <c r="I80" s="32"/>
     </row>
-    <row r="81" spans="1:9" ht="45">
+    <row r="81" spans="1:9" ht="30">
       <c r="A81" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B81" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C81" s="32" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D81" s="30"/>
       <c r="E81" s="30" t="s">
@@ -4283,13 +4349,13 @@
     </row>
     <row r="82" spans="1:9" ht="45">
       <c r="A82" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B82" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C82" s="32" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D82" s="30"/>
       <c r="E82" s="30" t="s">
@@ -4306,15 +4372,15 @@
       </c>
       <c r="I82" s="32"/>
     </row>
-    <row r="83" spans="1:9" ht="30">
+    <row r="83" spans="1:9" ht="45">
       <c r="A83" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B83" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C83" s="32" t="s">
-        <v>306</v>
+        <v>247</v>
       </c>
       <c r="D83" s="30"/>
       <c r="E83" s="30" t="s">
@@ -4331,15 +4397,15 @@
       </c>
       <c r="I83" s="32"/>
     </row>
-    <row r="84" spans="1:9" ht="45">
+    <row r="84" spans="1:9" ht="30">
       <c r="A84" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B84" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C84" s="32" t="s">
-        <v>251</v>
+        <v>300</v>
       </c>
       <c r="D84" s="30"/>
       <c r="E84" s="30" t="s">
@@ -4352,25 +4418,21 @@
         <v>15</v>
       </c>
       <c r="H84" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I84" s="32" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" ht="30">
+        <v>20</v>
+      </c>
+      <c r="I84" s="32"/>
+    </row>
+    <row r="85" spans="1:9" ht="45">
       <c r="A85" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B85" s="31" t="s">
         <v>32</v>
       </c>
       <c r="C85" s="32" t="s">
-        <v>313</v>
-      </c>
-      <c r="D85" s="30" t="s">
-        <v>287</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="D85" s="30"/>
       <c r="E85" s="30" t="s">
         <v>19</v>
       </c>
@@ -4381,21 +4443,25 @@
         <v>15</v>
       </c>
       <c r="H85" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I85" s="32"/>
-    </row>
-    <row r="86" spans="1:9" ht="45">
+        <v>17</v>
+      </c>
+      <c r="I85" s="32" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="30">
       <c r="A86" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B86" s="31" t="s">
-        <v>171</v>
+        <v>32</v>
       </c>
       <c r="C86" s="32" t="s">
-        <v>252</v>
-      </c>
-      <c r="D86" s="30"/>
+        <v>306</v>
+      </c>
+      <c r="D86" s="30" t="s">
+        <v>281</v>
+      </c>
       <c r="E86" s="30" t="s">
         <v>19</v>
       </c>
@@ -4406,25 +4472,21 @@
         <v>15</v>
       </c>
       <c r="H86" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I86" s="32" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="30">
+        <v>20</v>
+      </c>
+      <c r="I86" s="32"/>
+    </row>
+    <row r="87" spans="1:9" ht="45">
       <c r="A87" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B87" s="31" t="s">
         <v>171</v>
       </c>
       <c r="C87" s="32" t="s">
-        <v>307</v>
-      </c>
-      <c r="D87" s="30" t="s">
-        <v>288</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="D87" s="30"/>
       <c r="E87" s="30" t="s">
         <v>19</v>
       </c>
@@ -4435,21 +4497,25 @@
         <v>15</v>
       </c>
       <c r="H87" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I87" s="32"/>
-    </row>
-    <row r="88" spans="1:9" ht="45">
+        <v>17</v>
+      </c>
+      <c r="I87" s="32" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="30">
       <c r="A88" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B88" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C88" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="D88" s="30"/>
+        <v>301</v>
+      </c>
+      <c r="D88" s="30" t="s">
+        <v>282</v>
+      </c>
       <c r="E88" s="30" t="s">
         <v>19</v>
       </c>
@@ -4460,25 +4526,21 @@
         <v>15</v>
       </c>
       <c r="H88" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I88" s="32" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="30">
+        <v>20</v>
+      </c>
+      <c r="I88" s="32"/>
+    </row>
+    <row r="89" spans="1:9" ht="45">
       <c r="A89" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B89" s="31" t="s">
         <v>172</v>
       </c>
       <c r="C89" s="32" t="s">
-        <v>308</v>
-      </c>
-      <c r="D89" s="30" t="s">
-        <v>289</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="D89" s="30"/>
       <c r="E89" s="30" t="s">
         <v>19</v>
       </c>
@@ -4489,21 +4551,25 @@
         <v>15</v>
       </c>
       <c r="H89" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I89" s="32"/>
-    </row>
-    <row r="90" spans="1:9" ht="45">
+        <v>17</v>
+      </c>
+      <c r="I89" s="32" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="30">
       <c r="A90" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B90" s="31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C90" s="32" t="s">
-        <v>254</v>
-      </c>
-      <c r="D90" s="30"/>
+        <v>302</v>
+      </c>
+      <c r="D90" s="30" t="s">
+        <v>283</v>
+      </c>
       <c r="E90" s="30" t="s">
         <v>19</v>
       </c>
@@ -4514,25 +4580,21 @@
         <v>15</v>
       </c>
       <c r="H90" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I90" s="32" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="30">
+        <v>20</v>
+      </c>
+      <c r="I90" s="32"/>
+    </row>
+    <row r="91" spans="1:9" ht="45">
       <c r="A91" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B91" s="31" t="s">
         <v>173</v>
       </c>
       <c r="C91" s="32" t="s">
-        <v>309</v>
-      </c>
-      <c r="D91" s="30" t="s">
-        <v>290</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="D91" s="30"/>
       <c r="E91" s="30" t="s">
         <v>19</v>
       </c>
@@ -4543,21 +4605,25 @@
         <v>15</v>
       </c>
       <c r="H91" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I91" s="32"/>
-    </row>
-    <row r="92" spans="1:9" ht="45">
+        <v>17</v>
+      </c>
+      <c r="I91" s="32" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="30">
       <c r="A92" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C92" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="D92" s="30"/>
+        <v>303</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>284</v>
+      </c>
       <c r="E92" s="30" t="s">
         <v>19</v>
       </c>
@@ -4568,25 +4634,21 @@
         <v>15</v>
       </c>
       <c r="H92" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I92" s="32" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="30">
+        <v>20</v>
+      </c>
+      <c r="I92" s="32"/>
+    </row>
+    <row r="93" spans="1:9" ht="45">
       <c r="A93" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B93" s="31" t="s">
         <v>174</v>
       </c>
       <c r="C93" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="D93" s="30" t="s">
-        <v>291</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="D93" s="30"/>
       <c r="E93" s="30" t="s">
         <v>19</v>
       </c>
@@ -4597,21 +4659,25 @@
         <v>15</v>
       </c>
       <c r="H93" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I93" s="32"/>
-    </row>
-    <row r="94" spans="1:9" ht="45">
+        <v>17</v>
+      </c>
+      <c r="I93" s="32" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="30">
       <c r="A94" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B94" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C94" s="32" t="s">
-        <v>256</v>
-      </c>
-      <c r="D94" s="30"/>
+        <v>304</v>
+      </c>
+      <c r="D94" s="30" t="s">
+        <v>285</v>
+      </c>
       <c r="E94" s="30" t="s">
         <v>19</v>
       </c>
@@ -4622,25 +4688,21 @@
         <v>15</v>
       </c>
       <c r="H94" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I94" s="32" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="30">
+        <v>20</v>
+      </c>
+      <c r="I94" s="32"/>
+    </row>
+    <row r="95" spans="1:9" ht="45">
       <c r="A95" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B95" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="C95" s="32" t="s">
-        <v>311</v>
-      </c>
-      <c r="D95" s="30" t="s">
-        <v>292</v>
-      </c>
+      <c r="C95" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="D95" s="30"/>
       <c r="E95" s="30" t="s">
         <v>19</v>
       </c>
@@ -4651,21 +4713,25 @@
         <v>15</v>
       </c>
       <c r="H95" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I95" s="32"/>
-    </row>
-    <row r="96" spans="1:9" ht="45">
-      <c r="A96" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B96" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="C96" s="32" t="s">
-        <v>257</v>
-      </c>
-      <c r="D96" s="30"/>
+        <v>17</v>
+      </c>
+      <c r="I95" s="32" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="30">
+      <c r="A96" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="C96" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="D96" s="30" t="s">
+        <v>286</v>
+      </c>
       <c r="E96" s="30" t="s">
         <v>19</v>
       </c>
@@ -4676,25 +4742,21 @@
         <v>15</v>
       </c>
       <c r="H96" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I96" s="32" t="s">
-        <v>304</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I96" s="32"/>
     </row>
     <row r="97" spans="1:9" ht="30">
-      <c r="A97" s="30" t="s">
-        <v>119</v>
+      <c r="A97" s="22" t="s">
+        <v>316</v>
       </c>
       <c r="B97" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="C97" s="32" t="s">
-        <v>312</v>
-      </c>
-      <c r="D97" s="30" t="s">
-        <v>293</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="C97" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="D97" s="30"/>
       <c r="E97" s="30" t="s">
         <v>19</v>
       </c>
@@ -4709,42 +4771,46 @@
       </c>
       <c r="I97" s="32"/>
     </row>
-    <row r="98" spans="1:9" ht="30">
+    <row r="98" spans="1:9" ht="45">
       <c r="A98" s="30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B98" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C98" s="32" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D98" s="30"/>
       <c r="E98" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F98" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G98" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H98" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I98" s="32"/>
-    </row>
-    <row r="99" spans="1:9" ht="45">
-      <c r="A99" s="30" t="s">
-        <v>121</v>
+        <v>17</v>
+      </c>
+      <c r="I98" s="32" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="30">
+      <c r="A99" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C99" s="32" t="s">
-        <v>259</v>
-      </c>
-      <c r="D99" s="30"/>
+        <v>305</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>287</v>
+      </c>
       <c r="E99" s="30" t="s">
         <v>19</v>
       </c>
@@ -4760,14 +4826,14 @@
       <c r="I99" s="32"/>
     </row>
     <row r="100" spans="1:9" ht="45">
-      <c r="A100" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="B100" s="31" t="s">
+      <c r="A100" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="B100" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="C100" s="32" t="s">
-        <v>260</v>
+      <c r="C100" s="20" t="s">
+        <v>321</v>
       </c>
       <c r="D100" s="30"/>
       <c r="E100" s="30" t="s">
@@ -4780,21 +4846,25 @@
         <v>15</v>
       </c>
       <c r="H100" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I100" s="32"/>
-    </row>
-    <row r="101" spans="1:9" ht="60">
-      <c r="A101" s="30" t="s">
-        <v>123</v>
+        <v>17</v>
+      </c>
+      <c r="I100" s="20" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="30">
+      <c r="A101" s="22" t="s">
+        <v>322</v>
       </c>
       <c r="B101" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="C101" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="D101" s="30"/>
+      <c r="C101" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="D101" s="22" t="s">
+        <v>324</v>
+      </c>
       <c r="E101" s="30" t="s">
         <v>19</v>
       </c>
@@ -4809,22 +4879,22 @@
       </c>
       <c r="I101" s="32"/>
     </row>
-    <row r="102" spans="1:9" ht="75">
+    <row r="102" spans="1:9" ht="30">
       <c r="A102" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="B102" s="31" t="s">
-        <v>177</v>
+        <v>120</v>
+      </c>
+      <c r="B102" s="24" t="s">
+        <v>326</v>
       </c>
       <c r="C102" s="32" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="D102" s="30"/>
       <c r="E102" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F102" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G102" s="30" t="s">
         <v>15</v>
@@ -4834,15 +4904,15 @@
       </c>
       <c r="I102" s="32"/>
     </row>
-    <row r="103" spans="1:9" ht="75">
+    <row r="103" spans="1:9" ht="30">
       <c r="A103" s="30" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>177</v>
+        <v>326</v>
       </c>
       <c r="C103" s="32" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D103" s="30"/>
       <c r="E103" s="30" t="s">
@@ -4859,15 +4929,15 @@
       </c>
       <c r="I103" s="32"/>
     </row>
-    <row r="104" spans="1:9" ht="60">
+    <row r="104" spans="1:9" ht="45">
       <c r="A104" s="30" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>177</v>
+        <v>326</v>
       </c>
       <c r="C104" s="32" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D104" s="30"/>
       <c r="E104" s="30" t="s">
@@ -4884,15 +4954,15 @@
       </c>
       <c r="I104" s="32"/>
     </row>
-    <row r="105" spans="1:9" ht="60">
+    <row r="105" spans="1:9" ht="45">
       <c r="A105" s="30" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B105" s="31" t="s">
-        <v>177</v>
+        <v>326</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="D105" s="30"/>
       <c r="E105" s="30" t="s">
@@ -4905,19 +4975,19 @@
         <v>15</v>
       </c>
       <c r="H105" s="30" t="s">
-        <v>297</v>
+        <v>20</v>
       </c>
       <c r="I105" s="32"/>
     </row>
-    <row r="106" spans="1:9" ht="30">
+    <row r="106" spans="1:9" ht="60">
       <c r="A106" s="30" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B106" s="31" t="s">
-        <v>178</v>
+        <v>326</v>
       </c>
       <c r="C106" s="32" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D106" s="30"/>
       <c r="E106" s="30" t="s">
@@ -4930,19 +5000,19 @@
         <v>15</v>
       </c>
       <c r="H106" s="30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I106" s="32"/>
     </row>
-    <row r="107" spans="1:9" ht="30">
+    <row r="107" spans="1:9" ht="75">
       <c r="A107" s="30" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="C107" s="32" t="s">
-        <v>267</v>
+        <v>326</v>
+      </c>
+      <c r="C107" s="20" t="s">
+        <v>327</v>
       </c>
       <c r="D107" s="30"/>
       <c r="E107" s="30" t="s">
@@ -4955,119 +5025,119 @@
         <v>15</v>
       </c>
       <c r="H107" s="30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I107" s="32"/>
     </row>
-    <row r="108" spans="1:9" ht="30">
+    <row r="108" spans="1:9" ht="60">
       <c r="A108" s="30" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>180</v>
+        <v>326</v>
       </c>
       <c r="C108" s="32" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="D108" s="30"/>
       <c r="E108" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F108" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G108" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H108" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I108" s="32"/>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" ht="45">
       <c r="A109" s="30" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>181</v>
+        <v>326</v>
       </c>
       <c r="C109" s="32" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="D109" s="30"/>
       <c r="E109" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F109" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G109" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H109" s="30" t="s">
-        <v>18</v>
+        <v>291</v>
       </c>
       <c r="I109" s="32"/>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="30" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C110" s="32" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="D110" s="30"/>
       <c r="E110" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F110" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G110" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H110" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I110" s="32"/>
     </row>
-    <row r="111" spans="1:9" ht="30">
+    <row r="111" spans="1:9">
       <c r="A111" s="30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B111" s="31" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C111" s="32" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D111" s="30"/>
       <c r="E111" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F111" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G111" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H111" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I111" s="32"/>
     </row>
-    <row r="112" spans="1:9" ht="30">
+    <row r="112" spans="1:9">
       <c r="A112" s="30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B112" s="31" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C112" s="32" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="D112" s="30"/>
       <c r="E112" s="30" t="s">
@@ -5077,22 +5147,22 @@
         <v>7</v>
       </c>
       <c r="G112" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H112" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I112" s="32"/>
     </row>
-    <row r="113" spans="1:9" ht="30">
+    <row r="113" spans="1:9">
       <c r="A113" s="30" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B113" s="31" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C113" s="32" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="D113" s="30"/>
       <c r="E113" s="30" t="s">
@@ -5111,13 +5181,13 @@
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="30" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B114" s="31" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C114" s="32" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="D114" s="30"/>
       <c r="E114" s="30" t="s">
@@ -5136,13 +5206,13 @@
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="30" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B115" s="31" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="D115" s="30"/>
       <c r="E115" s="30" t="s">
@@ -5159,25 +5229,25 @@
       </c>
       <c r="I115" s="32"/>
     </row>
-    <row r="116" spans="1:9" ht="45">
+    <row r="116" spans="1:9" ht="30">
       <c r="A116" s="30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B116" s="31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C116" s="32" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="D116" s="30"/>
       <c r="E116" s="30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F116" s="30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G116" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H116" s="30" t="s">
         <v>18</v>
@@ -5186,42 +5256,42 @@
     </row>
     <row r="117" spans="1:9" ht="30">
       <c r="A117" s="30" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B117" s="31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C117" s="32" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D117" s="30"/>
       <c r="E117" s="30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F117" s="30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G117" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H117" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I117" s="32"/>
     </row>
-    <row r="118" spans="1:9" ht="30">
+    <row r="118" spans="1:9">
       <c r="A118" s="30" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C118" s="32" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="D118" s="30"/>
       <c r="E118" s="30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F118" s="30" t="s">
         <v>7</v>
@@ -5234,19 +5304,19 @@
       </c>
       <c r="I118" s="32"/>
     </row>
-    <row r="119" spans="1:9" ht="45">
+    <row r="119" spans="1:9">
       <c r="A119" s="30" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B119" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C119" s="32" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D119" s="30"/>
       <c r="E119" s="30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F119" s="30" t="s">
         <v>7</v>
@@ -5261,48 +5331,48 @@
     </row>
     <row r="120" spans="1:9" ht="45">
       <c r="A120" s="30" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B120" s="31" t="s">
         <v>187</v>
       </c>
       <c r="C120" s="32" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D120" s="30"/>
       <c r="E120" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F120" s="30" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G120" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H120" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I120" s="32"/>
     </row>
-    <row r="121" spans="1:9" ht="45">
+    <row r="121" spans="1:9" ht="30">
       <c r="A121" s="30" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B121" s="31" t="s">
         <v>187</v>
       </c>
       <c r="C121" s="32" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="D121" s="30"/>
       <c r="E121" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F121" s="30" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G121" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H121" s="30" t="s">
         <v>18</v>
@@ -5311,13 +5381,13 @@
     </row>
     <row r="122" spans="1:9" ht="30">
       <c r="A122" s="30" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B122" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="C122" s="32" t="s">
-        <v>282</v>
+      <c r="C122" s="20" t="s">
+        <v>328</v>
       </c>
       <c r="D122" s="30"/>
       <c r="E122" s="30" t="s">
@@ -5336,13 +5406,13 @@
     </row>
     <row r="123" spans="1:9" ht="45">
       <c r="A123" s="30" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B123" s="31" t="s">
         <v>187</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D123" s="30"/>
       <c r="E123" s="30" t="s">
@@ -5361,13 +5431,13 @@
     </row>
     <row r="124" spans="1:9" ht="30">
       <c r="A124" s="30" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B124" s="31" t="s">
         <v>187</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D124" s="30"/>
       <c r="E124" s="30" t="s">
@@ -5384,15 +5454,15 @@
       </c>
       <c r="I124" s="32"/>
     </row>
-    <row r="125" spans="1:9" ht="45">
+    <row r="125" spans="1:9" ht="30">
       <c r="A125" s="30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B125" s="31" t="s">
         <v>187</v>
       </c>
       <c r="C125" s="32" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D125" s="30"/>
       <c r="E125" s="30" t="s">
@@ -5411,13 +5481,13 @@
     </row>
     <row r="126" spans="1:9" ht="30">
       <c r="A126" s="30" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B126" s="31" t="s">
         <v>187</v>
       </c>
       <c r="C126" s="32" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D126" s="30"/>
       <c r="E126" s="30" t="s">
@@ -5434,72 +5504,177 @@
       </c>
       <c r="I126" s="32"/>
     </row>
-    <row r="127" spans="1:9" ht="60">
+    <row r="127" spans="1:9" ht="30">
       <c r="A127" s="30" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B127" s="31" t="s">
         <v>187</v>
       </c>
       <c r="C127" s="32" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
       <c r="D127" s="30"/>
       <c r="E127" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F127" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G127" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H127" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I127" s="32" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" ht="60">
+        <v>18</v>
+      </c>
+      <c r="I127" s="32"/>
+    </row>
+    <row r="128" spans="1:9" ht="30">
       <c r="A128" s="30" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B128" s="31" t="s">
         <v>187</v>
       </c>
       <c r="C128" s="32" t="s">
-        <v>315</v>
-      </c>
-      <c r="D128" s="30" t="s">
-        <v>294</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="D128" s="30"/>
       <c r="E128" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F128" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G128" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H128" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I128" s="32"/>
+    </row>
+    <row r="129" spans="1:9" ht="45">
+      <c r="A129" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="B129" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="C129" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="D129" s="30"/>
+      <c r="E129" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F129" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G129" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H129" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I129" s="32"/>
+    </row>
+    <row r="130" spans="1:9" ht="30">
+      <c r="A130" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="B130" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="C130" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="D130" s="30"/>
+      <c r="E130" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F130" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G130" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H130" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I130" s="32"/>
+    </row>
+    <row r="131" spans="1:9" ht="45">
+      <c r="A131" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="B131" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="C131" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="D131" s="30"/>
+      <c r="E131" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F131" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G128" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H128" s="30" t="s">
+      <c r="G131" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H131" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="I131" s="32" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="60">
+      <c r="A132" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="B132" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="C132" s="32" t="s">
+        <v>308</v>
+      </c>
+      <c r="D132" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="E132" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F132" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G132" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H132" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="I128" s="32" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
-      <c r="A129" s="3"/>
-      <c r="B129" s="10"/>
-    </row>
-    <row r="130" spans="1:2">
-      <c r="A130" s="3"/>
-      <c r="B130" s="10"/>
+      <c r="I132" s="32" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133" s="3"/>
+      <c r="B133" s="10"/>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" s="3"/>
+      <c r="B134" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -5507,14 +5682,9 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I20:I128 A20:H115 A34:I128">
+  <conditionalFormatting sqref="I20:I132 A20:H119 A34:I132">
     <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -5525,7 +5695,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I128 A20:H115 A34:I128">
+  <conditionalFormatting sqref="I20:I132 A20:H119 A34:I132">
     <cfRule type="expression" dxfId="23" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -5536,7 +5706,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F128">
+  <conditionalFormatting sqref="F20:F132">
     <cfRule type="expression" dxfId="20" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
@@ -5545,20 +5715,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F128">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F132">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E128">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E132">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G128">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G132">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H128">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H132">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5568,7 +5738,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B116:B130 C3 B10:B115" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B109:B134 B10:B108 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -5578,15 +5748,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -5635,6 +5796,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -5642,14 +5812,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5660,6 +5822,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[MS-WDVMODUU]: Update RS format
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WDVMODUU/MS-WDVMODUU_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WDVMODUU/MS-WDVMODUU_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -3422,7 +3422,7 @@
       </c>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" ht="30">
+    <row r="45" spans="1:9">
       <c r="A45" s="30" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
Update RS according to v20181001 document.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-WDVMODUU/MS-WDVMODUU_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-WDVMODUU/MS-WDVMODUU_RequirementSpecification.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites2\SharePoint\Docs\MS-WDVMODUU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\winboyer\Projects\VS_Project\hxc\Interop-TestSuites-1\SharePoint\Docs\MS-WDVMODUU\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="-15" yWindow="754" windowWidth="15403" windowHeight="6898" tabRatio="570"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -1277,16 +1277,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1482,13 +1482,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1521,7 +1521,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1584,7 +1584,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
     <dxf>
@@ -2146,7 +2146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2221,23 +2221,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2273,23 +2256,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2471,22 +2437,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.59765625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.73046875" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>289</v>
       </c>
@@ -2496,7 +2462,7 @@
       <c r="F1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>290</v>
       </c>
@@ -2507,22 +2473,22 @@
       <c r="F2" s="25"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="29">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>310</v>
       </c>
       <c r="F3" s="12">
-        <v>42566</v>
+        <v>43374</v>
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="21">
+    <row r="4" spans="1:10" ht="20.350000000000001" x14ac:dyDescent="0.45">
       <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
@@ -2534,7 +2500,7 @@
       <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
@@ -2550,7 +2516,7 @@
       <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
@@ -2566,7 +2532,7 @@
       <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
@@ -2582,7 +2548,7 @@
       <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
@@ -2598,7 +2564,7 @@
       <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="78.75" customHeight="1">
+    <row r="9" spans="1:10" ht="78.8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
@@ -2614,7 +2580,7 @@
       <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="33.75" customHeight="1">
+    <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
@@ -2630,7 +2596,7 @@
       <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
@@ -2646,7 +2612,7 @@
       <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
@@ -2664,7 +2630,7 @@
       <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
@@ -2682,7 +2648,7 @@
       <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="27" t="s">
         <v>7</v>
       </c>
@@ -2700,7 +2666,7 @@
       <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="28" t="s">
         <v>3</v>
       </c>
@@ -2718,7 +2684,7 @@
       <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1">
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
@@ -2734,7 +2700,7 @@
       <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="64.5" customHeight="1">
+    <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
@@ -2750,7 +2716,7 @@
       <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1">
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -2767,7 +2733,7 @@
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="30">
+    <row r="19" spans="1:12" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -2797,7 +2763,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="23" customFormat="1">
+    <row r="20" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>42</v>
       </c>
@@ -2822,7 +2788,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="28.65" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>43</v>
       </c>
@@ -2847,7 +2813,7 @@
       </c>
       <c r="I21" s="24"/>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="28.65" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>44</v>
       </c>
@@ -2872,7 +2838,7 @@
       </c>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:12" s="23" customFormat="1">
+    <row r="23" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>45</v>
       </c>
@@ -2897,7 +2863,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="28.65" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>46</v>
       </c>
@@ -2922,7 +2888,7 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1">
+    <row r="25" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>47</v>
       </c>
@@ -2947,7 +2913,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="26" spans="1:12" s="23" customFormat="1" ht="28.65" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>48</v>
       </c>
@@ -2972,7 +2938,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1">
+    <row r="27" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>49</v>
       </c>
@@ -2997,7 +2963,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="28.65" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>50</v>
       </c>
@@ -3022,7 +2988,7 @@
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="29" spans="1:12" s="23" customFormat="1" ht="28.65" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
         <v>51</v>
       </c>
@@ -3047,7 +3013,7 @@
       </c>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="30" spans="1:12" s="23" customFormat="1" ht="28.65" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
         <v>52</v>
       </c>
@@ -3072,7 +3038,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="31" spans="1:12" s="23" customFormat="1" ht="43" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>53</v>
       </c>
@@ -3097,7 +3063,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="32" spans="1:12" s="23" customFormat="1" ht="28.65" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
         <v>54</v>
       </c>
@@ -3122,7 +3088,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" ht="30">
+    <row r="33" spans="1:9" s="23" customFormat="1" ht="28.65" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
         <v>55</v>
       </c>
@@ -3147,7 +3113,7 @@
       </c>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" ht="30">
+    <row r="34" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A34" s="30" t="s">
         <v>56</v>
       </c>
@@ -3172,7 +3138,7 @@
       </c>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" ht="30">
+    <row r="35" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A35" s="30" t="s">
         <v>57</v>
       </c>
@@ -3197,7 +3163,7 @@
       </c>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9" ht="30">
+    <row r="36" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A36" s="30" t="s">
         <v>58</v>
       </c>
@@ -3222,7 +3188,7 @@
       </c>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9" ht="30">
+    <row r="37" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A37" s="30" t="s">
         <v>59</v>
       </c>
@@ -3247,7 +3213,7 @@
       </c>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="30" t="s">
         <v>60</v>
       </c>
@@ -3272,7 +3238,7 @@
       </c>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="30" t="s">
         <v>61</v>
       </c>
@@ -3297,7 +3263,7 @@
       </c>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9" ht="30">
+    <row r="40" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A40" s="30" t="s">
         <v>62</v>
       </c>
@@ -3322,7 +3288,7 @@
       </c>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" ht="30">
+    <row r="41" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A41" s="30" t="s">
         <v>63</v>
       </c>
@@ -3347,7 +3313,7 @@
       </c>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" ht="30">
+    <row r="42" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A42" s="30" t="s">
         <v>64</v>
       </c>
@@ -3372,7 +3338,7 @@
       </c>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" ht="30">
+    <row r="43" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A43" s="30" t="s">
         <v>65</v>
       </c>
@@ -3397,7 +3363,7 @@
       </c>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="30" t="s">
         <v>66</v>
       </c>
@@ -3422,7 +3388,7 @@
       </c>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A45" s="30" t="s">
         <v>67</v>
       </c>
@@ -3447,7 +3413,7 @@
       </c>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" ht="45">
+    <row r="46" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A46" s="30" t="s">
         <v>68</v>
       </c>
@@ -3472,7 +3438,7 @@
       </c>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" ht="30">
+    <row r="47" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A47" s="30" t="s">
         <v>69</v>
       </c>
@@ -3497,7 +3463,7 @@
       </c>
       <c r="I47" s="32"/>
     </row>
-    <row r="48" spans="1:9" ht="30">
+    <row r="48" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A48" s="30" t="s">
         <v>70</v>
       </c>
@@ -3522,7 +3488,7 @@
       </c>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9" ht="30">
+    <row r="49" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A49" s="30" t="s">
         <v>71</v>
       </c>
@@ -3547,7 +3513,7 @@
       </c>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" ht="30">
+    <row r="50" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A50" s="30" t="s">
         <v>72</v>
       </c>
@@ -3572,7 +3538,7 @@
       </c>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9" ht="30">
+    <row r="51" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A51" s="30" t="s">
         <v>73</v>
       </c>
@@ -3597,7 +3563,7 @@
       </c>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" ht="30">
+    <row r="52" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A52" s="30" t="s">
         <v>74</v>
       </c>
@@ -3622,7 +3588,7 @@
       </c>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" ht="30">
+    <row r="53" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A53" s="30" t="s">
         <v>75</v>
       </c>
@@ -3647,7 +3613,7 @@
       </c>
       <c r="I53" s="32"/>
     </row>
-    <row r="54" spans="1:9" ht="45">
+    <row r="54" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A54" s="30" t="s">
         <v>76</v>
       </c>
@@ -3672,7 +3638,7 @@
       </c>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9" ht="30">
+    <row r="55" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A55" s="30" t="s">
         <v>77</v>
       </c>
@@ -3697,7 +3663,7 @@
       </c>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A56" s="30" t="s">
         <v>78</v>
       </c>
@@ -3722,7 +3688,7 @@
       </c>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="30" t="s">
         <v>79</v>
       </c>
@@ -3747,7 +3713,7 @@
       </c>
       <c r="I57" s="32"/>
     </row>
-    <row r="58" spans="1:9" ht="45">
+    <row r="58" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A58" s="30" t="s">
         <v>80</v>
       </c>
@@ -3772,7 +3738,7 @@
       </c>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9" ht="30">
+    <row r="59" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A59" s="30" t="s">
         <v>81</v>
       </c>
@@ -3797,7 +3763,7 @@
       </c>
       <c r="I59" s="32"/>
     </row>
-    <row r="60" spans="1:9" ht="30">
+    <row r="60" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A60" s="30" t="s">
         <v>82</v>
       </c>
@@ -3822,7 +3788,7 @@
       </c>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9" ht="30">
+    <row r="61" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A61" s="30" t="s">
         <v>83</v>
       </c>
@@ -3847,7 +3813,7 @@
       </c>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" ht="45">
+    <row r="62" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A62" s="30" t="s">
         <v>84</v>
       </c>
@@ -3872,7 +3838,7 @@
       </c>
       <c r="I62" s="32"/>
     </row>
-    <row r="63" spans="1:9" ht="30">
+    <row r="63" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A63" s="30" t="s">
         <v>85</v>
       </c>
@@ -3897,7 +3863,7 @@
       </c>
       <c r="I63" s="32"/>
     </row>
-    <row r="64" spans="1:9" ht="30">
+    <row r="64" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A64" s="30" t="s">
         <v>86</v>
       </c>
@@ -3922,7 +3888,7 @@
       </c>
       <c r="I64" s="32"/>
     </row>
-    <row r="65" spans="1:9" ht="45">
+    <row r="65" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A65" s="22" t="s">
         <v>87</v>
       </c>
@@ -3947,7 +3913,7 @@
       </c>
       <c r="I65" s="32"/>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A66" s="30" t="s">
         <v>312</v>
       </c>
@@ -3972,7 +3938,7 @@
       </c>
       <c r="I66" s="32"/>
     </row>
-    <row r="67" spans="1:9" ht="45">
+    <row r="67" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A67" s="30" t="s">
         <v>88</v>
       </c>
@@ -3997,7 +3963,7 @@
       </c>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" ht="45">
+    <row r="68" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A68" s="30" t="s">
         <v>89</v>
       </c>
@@ -4022,7 +3988,7 @@
       </c>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="30">
+    <row r="69" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A69" s="30" t="s">
         <v>90</v>
       </c>
@@ -4047,7 +4013,7 @@
       </c>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A70" s="30" t="s">
         <v>91</v>
       </c>
@@ -4072,7 +4038,7 @@
       </c>
       <c r="I70" s="32"/>
     </row>
-    <row r="71" spans="1:9" ht="30">
+    <row r="71" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A71" s="30" t="s">
         <v>92</v>
       </c>
@@ -4097,7 +4063,7 @@
       </c>
       <c r="I71" s="32"/>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A72" s="30" t="s">
         <v>93</v>
       </c>
@@ -4122,7 +4088,7 @@
       </c>
       <c r="I72" s="32"/>
     </row>
-    <row r="73" spans="1:9" ht="30">
+    <row r="73" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A73" s="30" t="s">
         <v>94</v>
       </c>
@@ -4147,7 +4113,7 @@
       </c>
       <c r="I73" s="32"/>
     </row>
-    <row r="74" spans="1:9" ht="30">
+    <row r="74" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A74" s="30" t="s">
         <v>95</v>
       </c>
@@ -4172,7 +4138,7 @@
       </c>
       <c r="I74" s="32"/>
     </row>
-    <row r="75" spans="1:9" ht="30">
+    <row r="75" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A75" s="30" t="s">
         <v>96</v>
       </c>
@@ -4197,7 +4163,7 @@
       </c>
       <c r="I75" s="32"/>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="30" t="s">
         <v>97</v>
       </c>
@@ -4222,7 +4188,7 @@
       </c>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9" ht="30">
+    <row r="77" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A77" s="30" t="s">
         <v>98</v>
       </c>
@@ -4247,7 +4213,7 @@
       </c>
       <c r="I77" s="32"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="30" t="s">
         <v>99</v>
       </c>
@@ -4272,7 +4238,7 @@
       </c>
       <c r="I78" s="32"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="30" t="s">
         <v>100</v>
       </c>
@@ -4297,7 +4263,7 @@
       </c>
       <c r="I79" s="32"/>
     </row>
-    <row r="80" spans="1:9" ht="30">
+    <row r="80" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A80" s="30" t="s">
         <v>101</v>
       </c>
@@ -4322,7 +4288,7 @@
       </c>
       <c r="I80" s="32"/>
     </row>
-    <row r="81" spans="1:9" ht="30">
+    <row r="81" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A81" s="30" t="s">
         <v>102</v>
       </c>
@@ -4347,7 +4313,7 @@
       </c>
       <c r="I81" s="32"/>
     </row>
-    <row r="82" spans="1:9" ht="45">
+    <row r="82" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A82" s="30" t="s">
         <v>103</v>
       </c>
@@ -4372,7 +4338,7 @@
       </c>
       <c r="I82" s="32"/>
     </row>
-    <row r="83" spans="1:9" ht="45">
+    <row r="83" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A83" s="30" t="s">
         <v>104</v>
       </c>
@@ -4397,7 +4363,7 @@
       </c>
       <c r="I83" s="32"/>
     </row>
-    <row r="84" spans="1:9" ht="30">
+    <row r="84" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A84" s="30" t="s">
         <v>105</v>
       </c>
@@ -4422,7 +4388,7 @@
       </c>
       <c r="I84" s="32"/>
     </row>
-    <row r="85" spans="1:9" ht="45">
+    <row r="85" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A85" s="30" t="s">
         <v>106</v>
       </c>
@@ -4449,7 +4415,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30">
+    <row r="86" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A86" s="30" t="s">
         <v>107</v>
       </c>
@@ -4476,7 +4442,7 @@
       </c>
       <c r="I86" s="32"/>
     </row>
-    <row r="87" spans="1:9" ht="45">
+    <row r="87" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A87" s="30" t="s">
         <v>108</v>
       </c>
@@ -4503,7 +4469,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="30">
+    <row r="88" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A88" s="30" t="s">
         <v>109</v>
       </c>
@@ -4530,7 +4496,7 @@
       </c>
       <c r="I88" s="32"/>
     </row>
-    <row r="89" spans="1:9" ht="45">
+    <row r="89" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A89" s="30" t="s">
         <v>110</v>
       </c>
@@ -4557,7 +4523,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A90" s="30" t="s">
         <v>111</v>
       </c>
@@ -4584,7 +4550,7 @@
       </c>
       <c r="I90" s="32"/>
     </row>
-    <row r="91" spans="1:9" ht="45">
+    <row r="91" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A91" s="30" t="s">
         <v>112</v>
       </c>
@@ -4611,7 +4577,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="30">
+    <row r="92" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A92" s="30" t="s">
         <v>113</v>
       </c>
@@ -4638,7 +4604,7 @@
       </c>
       <c r="I92" s="32"/>
     </row>
-    <row r="93" spans="1:9" ht="45">
+    <row r="93" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A93" s="30" t="s">
         <v>114</v>
       </c>
@@ -4665,7 +4631,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="30">
+    <row r="94" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A94" s="30" t="s">
         <v>115</v>
       </c>
@@ -4692,7 +4658,7 @@
       </c>
       <c r="I94" s="32"/>
     </row>
-    <row r="95" spans="1:9" ht="45">
+    <row r="95" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A95" s="30" t="s">
         <v>116</v>
       </c>
@@ -4719,7 +4685,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="30">
+    <row r="96" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A96" s="22" t="s">
         <v>117</v>
       </c>
@@ -4746,7 +4712,7 @@
       </c>
       <c r="I96" s="32"/>
     </row>
-    <row r="97" spans="1:9" ht="30">
+    <row r="97" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A97" s="22" t="s">
         <v>316</v>
       </c>
@@ -4771,7 +4737,7 @@
       </c>
       <c r="I97" s="32"/>
     </row>
-    <row r="98" spans="1:9" ht="45">
+    <row r="98" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A98" s="30" t="s">
         <v>118</v>
       </c>
@@ -4798,7 +4764,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="30">
+    <row r="99" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A99" s="22" t="s">
         <v>119</v>
       </c>
@@ -4825,7 +4791,7 @@
       </c>
       <c r="I99" s="32"/>
     </row>
-    <row r="100" spans="1:9" ht="45">
+    <row r="100" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A100" s="22" t="s">
         <v>320</v>
       </c>
@@ -4852,7 +4818,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="30">
+    <row r="101" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A101" s="22" t="s">
         <v>322</v>
       </c>
@@ -4879,7 +4845,7 @@
       </c>
       <c r="I101" s="32"/>
     </row>
-    <row r="102" spans="1:9" ht="30">
+    <row r="102" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A102" s="30" t="s">
         <v>120</v>
       </c>
@@ -4904,7 +4870,7 @@
       </c>
       <c r="I102" s="32"/>
     </row>
-    <row r="103" spans="1:9" ht="30">
+    <row r="103" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A103" s="30" t="s">
         <v>121</v>
       </c>
@@ -4929,7 +4895,7 @@
       </c>
       <c r="I103" s="32"/>
     </row>
-    <row r="104" spans="1:9" ht="45">
+    <row r="104" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A104" s="30" t="s">
         <v>122</v>
       </c>
@@ -4954,7 +4920,7 @@
       </c>
       <c r="I104" s="32"/>
     </row>
-    <row r="105" spans="1:9" ht="45">
+    <row r="105" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A105" s="30" t="s">
         <v>123</v>
       </c>
@@ -4979,7 +4945,7 @@
       </c>
       <c r="I105" s="32"/>
     </row>
-    <row r="106" spans="1:9" ht="60">
+    <row r="106" spans="1:9" ht="57.3" x14ac:dyDescent="0.45">
       <c r="A106" s="30" t="s">
         <v>124</v>
       </c>
@@ -5004,7 +4970,7 @@
       </c>
       <c r="I106" s="32"/>
     </row>
-    <row r="107" spans="1:9" ht="75">
+    <row r="107" spans="1:9" ht="71.650000000000006" x14ac:dyDescent="0.45">
       <c r="A107" s="30" t="s">
         <v>125</v>
       </c>
@@ -5029,7 +4995,7 @@
       </c>
       <c r="I107" s="32"/>
     </row>
-    <row r="108" spans="1:9" ht="60">
+    <row r="108" spans="1:9" ht="57.3" x14ac:dyDescent="0.45">
       <c r="A108" s="30" t="s">
         <v>126</v>
       </c>
@@ -5054,7 +5020,7 @@
       </c>
       <c r="I108" s="32"/>
     </row>
-    <row r="109" spans="1:9" ht="45">
+    <row r="109" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A109" s="30" t="s">
         <v>127</v>
       </c>
@@ -5079,7 +5045,7 @@
       </c>
       <c r="I109" s="32"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" s="30" t="s">
         <v>128</v>
       </c>
@@ -5104,7 +5070,7 @@
       </c>
       <c r="I110" s="32"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" s="30" t="s">
         <v>129</v>
       </c>
@@ -5129,7 +5095,7 @@
       </c>
       <c r="I111" s="32"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A112" s="30" t="s">
         <v>130</v>
       </c>
@@ -5154,7 +5120,7 @@
       </c>
       <c r="I112" s="32"/>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="30" t="s">
         <v>131</v>
       </c>
@@ -5179,7 +5145,7 @@
       </c>
       <c r="I113" s="32"/>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" s="30" t="s">
         <v>132</v>
       </c>
@@ -5204,7 +5170,7 @@
       </c>
       <c r="I114" s="32"/>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" s="30" t="s">
         <v>133</v>
       </c>
@@ -5229,7 +5195,7 @@
       </c>
       <c r="I115" s="32"/>
     </row>
-    <row r="116" spans="1:9" ht="30">
+    <row r="116" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A116" s="30" t="s">
         <v>134</v>
       </c>
@@ -5254,7 +5220,7 @@
       </c>
       <c r="I116" s="32"/>
     </row>
-    <row r="117" spans="1:9" ht="30">
+    <row r="117" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A117" s="30" t="s">
         <v>135</v>
       </c>
@@ -5279,7 +5245,7 @@
       </c>
       <c r="I117" s="32"/>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" s="30" t="s">
         <v>136</v>
       </c>
@@ -5304,7 +5270,7 @@
       </c>
       <c r="I118" s="32"/>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" s="30" t="s">
         <v>137</v>
       </c>
@@ -5329,7 +5295,7 @@
       </c>
       <c r="I119" s="32"/>
     </row>
-    <row r="120" spans="1:9" ht="45">
+    <row r="120" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A120" s="30" t="s">
         <v>138</v>
       </c>
@@ -5354,7 +5320,7 @@
       </c>
       <c r="I120" s="32"/>
     </row>
-    <row r="121" spans="1:9" ht="30">
+    <row r="121" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A121" s="30" t="s">
         <v>139</v>
       </c>
@@ -5379,7 +5345,7 @@
       </c>
       <c r="I121" s="32"/>
     </row>
-    <row r="122" spans="1:9" ht="30">
+    <row r="122" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A122" s="30" t="s">
         <v>140</v>
       </c>
@@ -5404,7 +5370,7 @@
       </c>
       <c r="I122" s="32"/>
     </row>
-    <row r="123" spans="1:9" ht="45">
+    <row r="123" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A123" s="30" t="s">
         <v>141</v>
       </c>
@@ -5429,7 +5395,7 @@
       </c>
       <c r="I123" s="32"/>
     </row>
-    <row r="124" spans="1:9" ht="30">
+    <row r="124" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A124" s="30" t="s">
         <v>142</v>
       </c>
@@ -5454,7 +5420,7 @@
       </c>
       <c r="I124" s="32"/>
     </row>
-    <row r="125" spans="1:9" ht="30">
+    <row r="125" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A125" s="30" t="s">
         <v>143</v>
       </c>
@@ -5479,7 +5445,7 @@
       </c>
       <c r="I125" s="32"/>
     </row>
-    <row r="126" spans="1:9" ht="30">
+    <row r="126" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A126" s="30" t="s">
         <v>144</v>
       </c>
@@ -5504,7 +5470,7 @@
       </c>
       <c r="I126" s="32"/>
     </row>
-    <row r="127" spans="1:9" ht="30">
+    <row r="127" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A127" s="30" t="s">
         <v>145</v>
       </c>
@@ -5529,7 +5495,7 @@
       </c>
       <c r="I127" s="32"/>
     </row>
-    <row r="128" spans="1:9" ht="30">
+    <row r="128" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A128" s="30" t="s">
         <v>146</v>
       </c>
@@ -5554,7 +5520,7 @@
       </c>
       <c r="I128" s="32"/>
     </row>
-    <row r="129" spans="1:9" ht="45">
+    <row r="129" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A129" s="30" t="s">
         <v>147</v>
       </c>
@@ -5579,7 +5545,7 @@
       </c>
       <c r="I129" s="32"/>
     </row>
-    <row r="130" spans="1:9" ht="30">
+    <row r="130" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A130" s="30" t="s">
         <v>148</v>
       </c>
@@ -5604,7 +5570,7 @@
       </c>
       <c r="I130" s="32"/>
     </row>
-    <row r="131" spans="1:9" ht="45">
+    <row r="131" spans="1:9" ht="43" x14ac:dyDescent="0.45">
       <c r="A131" s="30" t="s">
         <v>149</v>
       </c>
@@ -5631,7 +5597,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="60">
+    <row r="132" spans="1:9" ht="57.3" x14ac:dyDescent="0.45">
       <c r="A132" s="30" t="s">
         <v>150</v>
       </c>
@@ -5660,11 +5626,11 @@
         <v>309</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" s="3"/>
       <c r="B133" s="10"/>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A134" s="3"/>
       <c r="B134" s="10"/>
     </row>
@@ -5738,7 +5704,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B109:B134 B10:B108 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B109:B134 B10:B108" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -5837,13 +5803,13 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>